<commit_message>
Added logger for all the info messages and refactored the code
</commit_message>
<xml_diff>
--- a/REST_MAIN/src/data/regDetails.xlsx
+++ b/REST_MAIN/src/data/regDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayakaushik\API_TRACK\REST_MAIN\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84A5FA1-6A96-49D5-9202-23B3DB64C350}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C4B0E0-281A-4B99-B401-509AF1D09F02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>aqwerty</t>
   </si>
   <si>
-    <t>masdadslaksdjlakjd@laskdjlaskjd.com</t>
+    <t>alkjfhlkajshdflkjblhjt!@asdasdas.acom</t>
   </si>
 </sst>
 </file>

</xml_diff>